<commit_message>
Fixing Book Online Tests
</commit_message>
<xml_diff>
--- a/Book_Online_001/Default.xlsx
+++ b/Book_Online_001/Default.xlsx
@@ -183,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="283845"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>